<commit_message>
excel upload done show data
</commit_message>
<xml_diff>
--- a/JobSeeker.xlsx
+++ b/JobSeeker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\JobConnector\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E548D74D-37D2-4AEC-8ED2-8481586E805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2938BF01-BF35-4E2A-A9F7-ABCE645BD2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>fullName</t>
   </si>
@@ -214,6 +214,36 @@
   </si>
   <si>
     <t>it developer</t>
+  </si>
+  <si>
+    <t>romiya</t>
+  </si>
+  <si>
+    <t>romiyaji@gmail.com</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>mahindra</t>
+  </si>
+  <si>
+    <t>http://example4/resume5.pdf</t>
+  </si>
+  <si>
+    <t>engineeer</t>
+  </si>
+  <si>
+    <t>somiya</t>
+  </si>
+  <si>
+    <t>somiyaji@gmail.com</t>
+  </si>
+  <si>
+    <t>http://example4/resumesomiya.pdf</t>
   </si>
 </sst>
 </file>
@@ -564,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +946,88 @@
         <v>62</v>
       </c>
     </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7965458569</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="2">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2500000</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3500000</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="5">
+        <v>45728</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6965458569</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2500000</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3500000</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="5">
+        <v>45728</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L4" r:id="rId1" xr:uid="{036DFD01-A2EF-48CE-9B0F-FD48BB0B7722}"/>
@@ -929,8 +1041,12 @@
     <hyperlink ref="L2" r:id="rId9" xr:uid="{76E30E8D-DD74-4A79-85C8-2C300783BE5C}"/>
     <hyperlink ref="C8" r:id="rId10" xr:uid="{BE449B39-55B4-408B-9FF4-A1375F58C8DE}"/>
     <hyperlink ref="L8" r:id="rId11" xr:uid="{26302FE2-3C43-43B4-98AF-479C6A7FA3FD}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{0E1D4F04-C8B7-4D52-8117-76A7656CAEAD}"/>
+    <hyperlink ref="L9" r:id="rId13" xr:uid="{54919841-B4D3-4600-B7E4-DF015211739A}"/>
+    <hyperlink ref="C10" r:id="rId14" xr:uid="{0093AA0E-E07B-43E7-8BE7-E6650A25A15C}"/>
+    <hyperlink ref="L10" r:id="rId15" xr:uid="{2CF189E1-4E20-48E8-82DD-D5E01420C79C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>